<commit_message>
minor correction of input dataset in DPE LISA P1 and creation of new mock data for GINI/LISA
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_LISA_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_LISA_P1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Projekte\NFDI4Health\TA5\Pilotprojekte\Harmonisierung\HarmonizR\use-cases-harmonisation\rmonize\data_proc_elem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FA1A5B-0FF7-4BAB-A7BE-EEB3CE25F0FD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF21D5A-D4CE-4865-AFA0-906A613E4F7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="394">
   <si>
     <t>index</t>
   </si>
@@ -1393,9 +1393,6 @@
   </si>
   <si>
     <t>Dietary Assessment Instrument</t>
-  </si>
-  <si>
-    <t>GINI_P1</t>
   </si>
   <si>
     <t>__BLANK__</t>
@@ -2400,8 +2397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2644,7 +2641,7 @@
         <v>25</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="15" t="s">
@@ -6570,19 +6567,19 @@
         <v>13</v>
       </c>
       <c r="E129" t="s">
+        <v>14</v>
+      </c>
+      <c r="F129" s="30" t="s">
         <v>390</v>
       </c>
-      <c r="F129" s="30" t="s">
+      <c r="G129" s="4" t="s">
         <v>391</v>
-      </c>
-      <c r="G129" s="4" t="s">
-        <v>392</v>
       </c>
       <c r="H129">
         <v>1</v>
       </c>
       <c r="I129" s="31" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J129" s="32" t="s">
         <v>16</v>
@@ -6614,15 +6611,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -6863,6 +6851,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBFC15CC-4CA5-447A-915F-1412CED97222}">
   <ds:schemaRefs>
@@ -6881,14 +6878,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA68FB6B-B5E6-4AB5-ACC7-06ACAB30D951}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6905,4 +6894,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
GL-4 DPE_LISA_P1+DPE_LISA_P2 updated EDU_LEVEL
</commit_message>
<xml_diff>
--- a/rmonize/data_proc_elem/DPE_LISA_P1.xlsx
+++ b/rmonize/data_proc_elem/DPE_LISA_P1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\rmonize\data_proc_elem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F54842-1D9A-4767-9CAD-1E9759DCC8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C4AFFB-BF15-49AD-B498-31C3584DB89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22260" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11025" yWindow="0" windowWidth="11025" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements_templa" sheetId="1" r:id="rId1"/>
@@ -1290,21 +1290,19 @@
   </si>
   <si>
     <t>case_when(
-      MUTBILD_0 == 1 &amp; VATBILD_0 == 1 ~ 0L,
-      MUTBILD_0 %in% c(2) | VATBILD_0 %in% c(2) ~ 1L,  
-      MUTBILD_0 %in% c(3) | VATBILD_0 %in% c(3) ~ 3L, 
-      MUTBILD_0 %in% c(4) | VATBILD_0 %in% c(4) ~ 2L, 
-      MUTBILD_0 %in% c(5, 6) | VATBILD_0 %in% c(5, 6) ~ 4L, 
-      MUTBILD_0 %in% c(7) | VATBILD_0 %in% c(7) ~ 5L,  
+      MUTBILD_0 %in% c(5, 6) | VATBILD_0 %in% c(5, 6) ~ 4L,
+      MUTBILD_0 %in% c(3,4) | VATBILD_0 %in% c(3,4) ~ 3L,
+      MUTBILD_0 %in% c(2) | VATBILD_0 %in% c(2) ~ 1L,
+      MUTBILD_0 == 1 | VATBILD_0 == 1 ~ 0L,
+      MUTBILD_0 %in% c(7) | VATBILD_0 %in% c(7) ~ 5L,
       TRUE ~ NA_integer_
     )</t>
   </si>
   <si>
-    <t>"None" (0): Both parents have 1 (no certificate).
+    <t>"Longer Education" (4): Either parent has 5 or 6.
+"Secondary School" (3): Either parent has 3 or 4.
 "Primary School Completed" (1): Either parent has 2.
-"Technical/Professional School" (2): Either parent has 4.
-"Secondary School" (3): Either parent has 3.
-"Longer Education" (4): Either parent has 5 or 6.
+"None" (0): Either parent has 1 (no certificate).
 "Not Specified" (5): Either parent has 7 (other degree).</t>
   </si>
 </sst>
@@ -1899,7 +1897,7 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2260,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2411,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="255" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6464,6 +6462,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -6704,15 +6711,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -6726,6 +6724,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA68FB6B-B5E6-4AB5-ACC7-06ACAB30D951}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6740,14 +6746,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E89B3EC5-962B-41D9-9821-3A191D2434CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>